<commit_message>
Report writing and testing with variable voltage
</commit_message>
<xml_diff>
--- a/50kHz measurments.xlsx
+++ b/50kHz measurments.xlsx
@@ -8,28 +8,18 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ksmall1\Documents\GitHub\PROJ324_SK\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6FCC8DD-5DE7-48E0-9477-8322340C6E6F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B32BAFB-A131-4879-92CA-CB480EA430C8}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{49929126-E106-4BA5-BBBE-362DD2DFA756}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -3528,6 +3518,921 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" spc="120" normalizeH="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="diamond"/>
+            <c:size val="6"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="9525" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet2!$D$5:$D$50</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="46"/>
+                <c:pt idx="0">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>21</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>23</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>26</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>27</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>29</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>31</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>33</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>34</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>36</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>37</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>38</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>39</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>41</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>42</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>43</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>44</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>45</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>55</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>65</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>70</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet2!$F$10:$F$50</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="41"/>
+                <c:pt idx="0">
+                  <c:v>195.10199999999998</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>216.51099999999997</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>231.21199999999999</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>240.02299999999991</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>244.24900000000002</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>245.2940000000001</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>222.16600000000005</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>205.54399999999998</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>218.72899999999981</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>215.88599999999997</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>252.596</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>250.07500000000005</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>285.78700000000003</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>298.83200000000011</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>305.09800000000018</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>315.53799999999978</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>301.49</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>300.24299999999994</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>278.59999999999991</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>263.41200000000003</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>284.48800000000006</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>284.15700000000015</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>320.5450000000003</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>343.60099999999989</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>364.47199999999975</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>384.94299999999998</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>349.82400000000007</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>323.54599999999982</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>305.55099999999993</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>316.41300000000001</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>307.82899999999972</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>319.94500000000016</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>314.49400000000014</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>337.73199999999997</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>364.45299999999997</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>426.52700000000004</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>364.54899999999998</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>358.19399999999996</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>385.74000000000024</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>375.58000000000038</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>416.8119999999999</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-7A01-427E-9E6C-2F4848D6E32E}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="square"/>
+            <c:size val="6"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="9525" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet2!$D$5:$D$50</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="46"/>
+                <c:pt idx="0">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>21</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>23</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>26</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>27</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>29</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>31</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>33</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>34</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>36</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>37</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>38</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>39</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>41</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>42</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>43</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>44</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>45</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>55</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>65</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>70</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet2!$C$5:$C$44</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="40"/>
+                <c:pt idx="0">
+                  <c:v>211.90999999999997</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>196.92400000000004</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>188.90800000000002</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>182.447</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>181.90500000000009</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>150.255</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>193.37900000000002</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>216.43299999999999</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>239.41699999999992</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>251.18900000000008</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>258.28199999999993</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>260.43899999999996</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>255.95899999999995</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>243.09399999999982</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>234.28999999999996</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>240.25199999999995</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>243.86300000000006</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>275.53099999999995</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>298.31600000000003</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>308.15900000000011</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>323.97999999999979</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>317.59199999999987</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>310.42399999999998</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>308.53700000000003</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>260.70399999999995</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>284.29500000000007</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>283.66200000000026</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>293.9190000000001</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>295.02299999999991</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>290.97699999999986</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>371.92100000000005</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>348.65700000000015</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>382.42599999999993</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>355.92300000000023</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>337.33199999999988</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>313.84999999999991</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>316.55200000000013</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>336.74499999999989</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>348.59099999999989</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>390.76600000000008</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-7A01-427E-9E6C-2F4848D6E32E}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="1196160384"/>
+        <c:axId val="1093146800"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="1196160384"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="all" spc="120" normalizeH="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1093146800"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="1093146800"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="dk1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1196160384"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="lt1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -3688,6 +4593,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
@@ -5237,6 +6182,526 @@
 </file>
 
 <file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="241">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200" cap="all"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200" cap="all" spc="120" normalizeH="0" baseline="0"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="50000"/>
+        <a:lumOff val="50000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="22225" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout size="6"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1600" b="1" kern="1200" cap="all" spc="120" normalizeH="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="800" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style5.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="241">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -5897,6 +7362,47 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>581024</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>147637</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>361949</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{71FC93AE-4AC8-45D8-B3FA-183D25CC5BC7}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -6204,8 +7710,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7288C5F0-AF61-4E26-9BFE-C4E1DAB9DA45}">
   <dimension ref="A2:V47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="D52" sqref="D52"/>
+    <sheetView tabSelected="1" topLeftCell="G25" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7218,4 +8724,965 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7A581574-D065-4677-A136-CE1820FEC8BC}">
+  <dimension ref="A5:F51"/>
+  <sheetViews>
+    <sheetView topLeftCell="K6" workbookViewId="0">
+      <selection activeCell="F52" sqref="F52"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>291.54500000000002</v>
+      </c>
+      <c r="B5">
+        <v>503.45499999999998</v>
+      </c>
+      <c r="C5">
+        <f>B5-A5</f>
+        <v>211.90999999999997</v>
+      </c>
+      <c r="D5">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>349.85399999999998</v>
+      </c>
+      <c r="B6">
+        <v>546.77800000000002</v>
+      </c>
+      <c r="C6">
+        <f t="shared" ref="C6:C44" si="0">B6-A6</f>
+        <v>196.92400000000004</v>
+      </c>
+      <c r="D6">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>408.16300000000001</v>
+      </c>
+      <c r="B7">
+        <v>597.07100000000003</v>
+      </c>
+      <c r="C7">
+        <f t="shared" si="0"/>
+        <v>188.90800000000002</v>
+      </c>
+      <c r="D7">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>466.47199999999998</v>
+      </c>
+      <c r="B8">
+        <v>648.91899999999998</v>
+      </c>
+      <c r="C8">
+        <f t="shared" si="0"/>
+        <v>182.447</v>
+      </c>
+      <c r="D8">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>524.78099999999995</v>
+      </c>
+      <c r="B9">
+        <v>706.68600000000004</v>
+      </c>
+      <c r="C9">
+        <f t="shared" si="0"/>
+        <v>181.90500000000009</v>
+      </c>
+      <c r="D9">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>583.09</v>
+      </c>
+      <c r="B10">
+        <v>733.34500000000003</v>
+      </c>
+      <c r="C10">
+        <f t="shared" si="0"/>
+        <v>150.255</v>
+      </c>
+      <c r="D10">
+        <v>10</v>
+      </c>
+      <c r="E10">
+        <v>778.19200000000001</v>
+      </c>
+      <c r="F10">
+        <f>E10-A10</f>
+        <v>195.10199999999998</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>641.399</v>
+      </c>
+      <c r="B11">
+        <v>834.77800000000002</v>
+      </c>
+      <c r="C11">
+        <f t="shared" si="0"/>
+        <v>193.37900000000002</v>
+      </c>
+      <c r="D11">
+        <v>11</v>
+      </c>
+      <c r="E11">
+        <v>857.91</v>
+      </c>
+      <c r="F11">
+        <f t="shared" ref="F11:F50" si="1">E11-A11</f>
+        <v>216.51099999999997</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>699.70799999999997</v>
+      </c>
+      <c r="B12">
+        <v>916.14099999999996</v>
+      </c>
+      <c r="C12">
+        <f t="shared" si="0"/>
+        <v>216.43299999999999</v>
+      </c>
+      <c r="D12">
+        <v>12</v>
+      </c>
+      <c r="E12">
+        <v>930.92</v>
+      </c>
+      <c r="F12">
+        <f t="shared" si="1"/>
+        <v>231.21199999999999</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>758.01700000000005</v>
+      </c>
+      <c r="B13">
+        <v>997.43399999999997</v>
+      </c>
+      <c r="C13">
+        <f t="shared" si="0"/>
+        <v>239.41699999999992</v>
+      </c>
+      <c r="D13">
+        <v>13</v>
+      </c>
+      <c r="E13">
+        <v>998.04</v>
+      </c>
+      <c r="F13">
+        <f t="shared" si="1"/>
+        <v>240.02299999999991</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>816.327</v>
+      </c>
+      <c r="B14">
+        <v>1067.5160000000001</v>
+      </c>
+      <c r="C14">
+        <f t="shared" si="0"/>
+        <v>251.18900000000008</v>
+      </c>
+      <c r="D14">
+        <v>14</v>
+      </c>
+      <c r="E14">
+        <v>1060.576</v>
+      </c>
+      <c r="F14">
+        <f t="shared" si="1"/>
+        <v>244.24900000000002</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>874.63599999999997</v>
+      </c>
+      <c r="B15">
+        <v>1132.9179999999999</v>
+      </c>
+      <c r="C15">
+        <f t="shared" si="0"/>
+        <v>258.28199999999993</v>
+      </c>
+      <c r="D15">
+        <v>15</v>
+      </c>
+      <c r="E15">
+        <v>1119.93</v>
+      </c>
+      <c r="F15">
+        <f t="shared" si="1"/>
+        <v>245.2940000000001</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>932.94500000000005</v>
+      </c>
+      <c r="B16">
+        <v>1193.384</v>
+      </c>
+      <c r="C16">
+        <f t="shared" si="0"/>
+        <v>260.43899999999996</v>
+      </c>
+      <c r="D16">
+        <v>16</v>
+      </c>
+      <c r="E16">
+        <v>1155.1110000000001</v>
+      </c>
+      <c r="F16">
+        <f t="shared" si="1"/>
+        <v>222.16600000000005</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>991.25400000000002</v>
+      </c>
+      <c r="B17">
+        <v>1247.213</v>
+      </c>
+      <c r="C17">
+        <f t="shared" si="0"/>
+        <v>255.95899999999995</v>
+      </c>
+      <c r="D17">
+        <v>17</v>
+      </c>
+      <c r="E17">
+        <v>1196.798</v>
+      </c>
+      <c r="F17">
+        <f t="shared" si="1"/>
+        <v>205.54399999999998</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>1049.5630000000001</v>
+      </c>
+      <c r="B18">
+        <v>1292.6569999999999</v>
+      </c>
+      <c r="C18">
+        <f t="shared" si="0"/>
+        <v>243.09399999999982</v>
+      </c>
+      <c r="D18">
+        <v>18</v>
+      </c>
+      <c r="E18">
+        <v>1268.2919999999999</v>
+      </c>
+      <c r="F18">
+        <f t="shared" si="1"/>
+        <v>218.72899999999981</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>1107.8720000000001</v>
+      </c>
+      <c r="B19">
+        <v>1342.162</v>
+      </c>
+      <c r="C19">
+        <f t="shared" si="0"/>
+        <v>234.28999999999996</v>
+      </c>
+      <c r="D19">
+        <v>19</v>
+      </c>
+      <c r="E19">
+        <v>1323.758</v>
+      </c>
+      <c r="F19">
+        <f t="shared" si="1"/>
+        <v>215.88599999999997</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>1166.181</v>
+      </c>
+      <c r="B20">
+        <v>1406.433</v>
+      </c>
+      <c r="C20">
+        <f t="shared" si="0"/>
+        <v>240.25199999999995</v>
+      </c>
+      <c r="D20">
+        <v>20</v>
+      </c>
+      <c r="E20">
+        <v>1418.777</v>
+      </c>
+      <c r="F20">
+        <f t="shared" si="1"/>
+        <v>252.596</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>1224.49</v>
+      </c>
+      <c r="B21">
+        <v>1468.3530000000001</v>
+      </c>
+      <c r="C21">
+        <f t="shared" si="0"/>
+        <v>243.86300000000006</v>
+      </c>
+      <c r="D21">
+        <v>21</v>
+      </c>
+      <c r="E21">
+        <v>1474.5650000000001</v>
+      </c>
+      <c r="F21">
+        <f t="shared" si="1"/>
+        <v>250.07500000000005</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>1282.799</v>
+      </c>
+      <c r="B22">
+        <v>1558.33</v>
+      </c>
+      <c r="C22">
+        <f t="shared" si="0"/>
+        <v>275.53099999999995</v>
+      </c>
+      <c r="D22">
+        <v>22</v>
+      </c>
+      <c r="E22">
+        <v>1568.586</v>
+      </c>
+      <c r="F22">
+        <f t="shared" si="1"/>
+        <v>285.78700000000003</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>1341.1079999999999</v>
+      </c>
+      <c r="B23">
+        <v>1639.424</v>
+      </c>
+      <c r="C23">
+        <f t="shared" si="0"/>
+        <v>298.31600000000003</v>
+      </c>
+      <c r="D23">
+        <v>23</v>
+      </c>
+      <c r="E23">
+        <v>1639.94</v>
+      </c>
+      <c r="F23">
+        <f t="shared" si="1"/>
+        <v>298.83200000000011</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>1399.4169999999999</v>
+      </c>
+      <c r="B24">
+        <v>1707.576</v>
+      </c>
+      <c r="C24">
+        <f t="shared" si="0"/>
+        <v>308.15900000000011</v>
+      </c>
+      <c r="D24">
+        <v>24</v>
+      </c>
+      <c r="E24">
+        <v>1704.5150000000001</v>
+      </c>
+      <c r="F24">
+        <f t="shared" si="1"/>
+        <v>305.09800000000018</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>1457.7260000000001</v>
+      </c>
+      <c r="B25">
+        <v>1781.7059999999999</v>
+      </c>
+      <c r="C25">
+        <f t="shared" si="0"/>
+        <v>323.97999999999979</v>
+      </c>
+      <c r="D25">
+        <v>25</v>
+      </c>
+      <c r="E25">
+        <v>1773.2639999999999</v>
+      </c>
+      <c r="F25">
+        <f t="shared" si="1"/>
+        <v>315.53799999999978</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>1516.0350000000001</v>
+      </c>
+      <c r="B26">
+        <v>1833.627</v>
+      </c>
+      <c r="C26">
+        <f t="shared" si="0"/>
+        <v>317.59199999999987</v>
+      </c>
+      <c r="D26">
+        <v>26</v>
+      </c>
+      <c r="E26">
+        <v>1817.5250000000001</v>
+      </c>
+      <c r="F26">
+        <f t="shared" si="1"/>
+        <v>301.49</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>1574.3440000000001</v>
+      </c>
+      <c r="B27">
+        <v>1884.768</v>
+      </c>
+      <c r="C27">
+        <f t="shared" si="0"/>
+        <v>310.42399999999998</v>
+      </c>
+      <c r="D27">
+        <v>27</v>
+      </c>
+      <c r="E27">
+        <v>1874.587</v>
+      </c>
+      <c r="F27">
+        <f t="shared" si="1"/>
+        <v>300.24299999999994</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>1632.653</v>
+      </c>
+      <c r="B28">
+        <v>1941.19</v>
+      </c>
+      <c r="C28">
+        <f t="shared" si="0"/>
+        <v>308.53700000000003</v>
+      </c>
+      <c r="D28">
+        <v>28</v>
+      </c>
+      <c r="E28">
+        <v>1911.2529999999999</v>
+      </c>
+      <c r="F28">
+        <f t="shared" si="1"/>
+        <v>278.59999999999991</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>1690.962</v>
+      </c>
+      <c r="B29">
+        <v>1951.6659999999999</v>
+      </c>
+      <c r="C29">
+        <f t="shared" si="0"/>
+        <v>260.70399999999995</v>
+      </c>
+      <c r="D29">
+        <v>29</v>
+      </c>
+      <c r="E29">
+        <v>1954.374</v>
+      </c>
+      <c r="F29">
+        <f t="shared" si="1"/>
+        <v>263.41200000000003</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>1749.271</v>
+      </c>
+      <c r="B30">
+        <v>2033.566</v>
+      </c>
+      <c r="C30">
+        <f t="shared" si="0"/>
+        <v>284.29500000000007</v>
+      </c>
+      <c r="D30">
+        <v>30</v>
+      </c>
+      <c r="E30">
+        <v>2033.759</v>
+      </c>
+      <c r="F30">
+        <f t="shared" si="1"/>
+        <v>284.48800000000006</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>1807.58</v>
+      </c>
+      <c r="B31">
+        <v>2091.2420000000002</v>
+      </c>
+      <c r="C31">
+        <f t="shared" si="0"/>
+        <v>283.66200000000026</v>
+      </c>
+      <c r="D31">
+        <v>31</v>
+      </c>
+      <c r="E31">
+        <v>2091.7370000000001</v>
+      </c>
+      <c r="F31">
+        <f t="shared" si="1"/>
+        <v>284.15700000000015</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>1865.8889999999999</v>
+      </c>
+      <c r="B32">
+        <v>2159.808</v>
+      </c>
+      <c r="C32">
+        <f t="shared" si="0"/>
+        <v>293.9190000000001</v>
+      </c>
+      <c r="D32">
+        <v>32</v>
+      </c>
+      <c r="E32">
+        <v>2186.4340000000002</v>
+      </c>
+      <c r="F32">
+        <f t="shared" si="1"/>
+        <v>320.5450000000003</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>1924.1980000000001</v>
+      </c>
+      <c r="B33">
+        <v>2219.221</v>
+      </c>
+      <c r="C33">
+        <f t="shared" si="0"/>
+        <v>295.02299999999991</v>
+      </c>
+      <c r="D33">
+        <v>33</v>
+      </c>
+      <c r="E33">
+        <v>2267.799</v>
+      </c>
+      <c r="F33">
+        <f t="shared" si="1"/>
+        <v>343.60099999999989</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>1982.5070000000001</v>
+      </c>
+      <c r="B34">
+        <v>2273.4839999999999</v>
+      </c>
+      <c r="C34">
+        <f t="shared" si="0"/>
+        <v>290.97699999999986</v>
+      </c>
+      <c r="D34">
+        <v>34</v>
+      </c>
+      <c r="E34">
+        <v>2346.9789999999998</v>
+      </c>
+      <c r="F34">
+        <f t="shared" si="1"/>
+        <v>364.47199999999975</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>2040.816</v>
+      </c>
+      <c r="B35">
+        <v>2412.7370000000001</v>
+      </c>
+      <c r="C35">
+        <f t="shared" si="0"/>
+        <v>371.92100000000005</v>
+      </c>
+      <c r="D35">
+        <v>35</v>
+      </c>
+      <c r="E35">
+        <v>2425.759</v>
+      </c>
+      <c r="F35">
+        <f t="shared" si="1"/>
+        <v>384.94299999999998</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <v>2099.125</v>
+      </c>
+      <c r="B36">
+        <v>2447.7820000000002</v>
+      </c>
+      <c r="C36">
+        <f t="shared" si="0"/>
+        <v>348.65700000000015</v>
+      </c>
+      <c r="D36">
+        <v>36</v>
+      </c>
+      <c r="E36">
+        <v>2448.9490000000001</v>
+      </c>
+      <c r="F36">
+        <f t="shared" si="1"/>
+        <v>349.82400000000007</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <v>2157.4340000000002</v>
+      </c>
+      <c r="B37">
+        <v>2539.86</v>
+      </c>
+      <c r="C37">
+        <f t="shared" si="0"/>
+        <v>382.42599999999993</v>
+      </c>
+      <c r="D37">
+        <v>37</v>
+      </c>
+      <c r="E37">
+        <v>2480.98</v>
+      </c>
+      <c r="F37">
+        <f t="shared" si="1"/>
+        <v>323.54599999999982</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A38">
+        <v>2215.7429999999999</v>
+      </c>
+      <c r="B38">
+        <v>2571.6660000000002</v>
+      </c>
+      <c r="C38">
+        <f t="shared" si="0"/>
+        <v>355.92300000000023</v>
+      </c>
+      <c r="D38">
+        <v>38</v>
+      </c>
+      <c r="E38">
+        <v>2521.2939999999999</v>
+      </c>
+      <c r="F38">
+        <f t="shared" si="1"/>
+        <v>305.55099999999993</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A39">
+        <v>2274.0520000000001</v>
+      </c>
+      <c r="B39">
+        <v>2611.384</v>
+      </c>
+      <c r="C39">
+        <f t="shared" si="0"/>
+        <v>337.33199999999988</v>
+      </c>
+      <c r="D39">
+        <v>39</v>
+      </c>
+      <c r="E39">
+        <v>2590.4650000000001</v>
+      </c>
+      <c r="F39">
+        <f t="shared" si="1"/>
+        <v>316.41300000000001</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A40">
+        <v>2332.3620000000001</v>
+      </c>
+      <c r="B40">
+        <v>2646.212</v>
+      </c>
+      <c r="C40">
+        <f t="shared" si="0"/>
+        <v>313.84999999999991</v>
+      </c>
+      <c r="D40">
+        <v>40</v>
+      </c>
+      <c r="E40">
+        <v>2640.1909999999998</v>
+      </c>
+      <c r="F40">
+        <f t="shared" si="1"/>
+        <v>307.82899999999972</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A41">
+        <v>2390.6709999999998</v>
+      </c>
+      <c r="B41">
+        <v>2707.223</v>
+      </c>
+      <c r="C41">
+        <f t="shared" si="0"/>
+        <v>316.55200000000013</v>
+      </c>
+      <c r="D41">
+        <v>41</v>
+      </c>
+      <c r="E41">
+        <v>2710.616</v>
+      </c>
+      <c r="F41">
+        <f t="shared" si="1"/>
+        <v>319.94500000000016</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A42">
+        <v>2448.98</v>
+      </c>
+      <c r="B42">
+        <v>2785.7249999999999</v>
+      </c>
+      <c r="C42">
+        <f t="shared" si="0"/>
+        <v>336.74499999999989</v>
+      </c>
+      <c r="D42">
+        <v>42</v>
+      </c>
+      <c r="E42">
+        <v>2763.4740000000002</v>
+      </c>
+      <c r="F42">
+        <f t="shared" si="1"/>
+        <v>314.49400000000014</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A43">
+        <v>2507.2890000000002</v>
+      </c>
+      <c r="B43">
+        <v>2855.88</v>
+      </c>
+      <c r="C43">
+        <f t="shared" si="0"/>
+        <v>348.59099999999989</v>
+      </c>
+      <c r="D43">
+        <v>43</v>
+      </c>
+      <c r="E43">
+        <v>2845.0210000000002</v>
+      </c>
+      <c r="F43">
+        <f t="shared" si="1"/>
+        <v>337.73199999999997</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A44">
+        <v>2565.598</v>
+      </c>
+      <c r="B44">
+        <v>2956.364</v>
+      </c>
+      <c r="C44">
+        <f t="shared" si="0"/>
+        <v>390.76600000000008</v>
+      </c>
+      <c r="D44">
+        <v>44</v>
+      </c>
+      <c r="E44">
+        <v>2930.0509999999999</v>
+      </c>
+      <c r="F44">
+        <f t="shared" si="1"/>
+        <v>364.45299999999997</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A45">
+        <v>2623.9070000000002</v>
+      </c>
+      <c r="C45">
+        <f>AVERAGE(C5:C44)</f>
+        <v>277.57070000000004</v>
+      </c>
+      <c r="D45">
+        <v>45</v>
+      </c>
+      <c r="E45">
+        <v>3050.4340000000002</v>
+      </c>
+      <c r="F45">
+        <f t="shared" si="1"/>
+        <v>426.52700000000004</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A46">
+        <v>2915.4520000000002</v>
+      </c>
+      <c r="D46">
+        <v>50</v>
+      </c>
+      <c r="E46">
+        <v>3280.0010000000002</v>
+      </c>
+      <c r="F46">
+        <f t="shared" si="1"/>
+        <v>364.54899999999998</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A47">
+        <v>3206.9969999999998</v>
+      </c>
+      <c r="D47">
+        <v>55</v>
+      </c>
+      <c r="E47">
+        <v>3565.1909999999998</v>
+      </c>
+      <c r="F47">
+        <f t="shared" si="1"/>
+        <v>358.19399999999996</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A48">
+        <v>3498.5419999999999</v>
+      </c>
+      <c r="D48">
+        <v>60</v>
+      </c>
+      <c r="E48">
+        <v>3884.2820000000002</v>
+      </c>
+      <c r="F48">
+        <f t="shared" si="1"/>
+        <v>385.74000000000024</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A49">
+        <v>3790.087</v>
+      </c>
+      <c r="D49">
+        <v>65</v>
+      </c>
+      <c r="E49">
+        <v>4165.6670000000004</v>
+      </c>
+      <c r="F49">
+        <f t="shared" si="1"/>
+        <v>375.58000000000038</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A50">
+        <v>4081.6329999999998</v>
+      </c>
+      <c r="D50">
+        <v>70</v>
+      </c>
+      <c r="E50">
+        <v>4498.4449999999997</v>
+      </c>
+      <c r="F50">
+        <f t="shared" si="1"/>
+        <v>416.8119999999999</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F51">
+        <f>AVERAGE(F10:F46)</f>
+        <v>291.87718918918927</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
report writing and some research/sims
</commit_message>
<xml_diff>
--- a/50kHz measurments.xlsx
+++ b/50kHz measurments.xlsx
@@ -8,14 +8,19 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ksmall1\Documents\GitHub\PROJ324_SK\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B32BAFB-A131-4879-92CA-CB480EA430C8}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A48811E-DB94-455A-AB2D-8F7525A32125}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{49929126-E106-4BA5-BBBE-362DD2DFA756}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{49929126-E106-4BA5-BBBE-362DD2DFA756}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId2"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId3"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlchart.v1.0" hidden="1">Sheet3!$A$5:$A$30</definedName>
+    <definedName name="_xlchart.v1.1" hidden="1">Sheet3!$B$5:$B$30</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -3546,6 +3551,460 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="5.8991896160600729E-2"/>
+          <c:y val="0.12845021645021645"/>
+          <c:w val="0.90841198403500201"/>
+          <c:h val="0.79120946245355694"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet3!$A$5:$A$30</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="26"/>
+                <c:pt idx="0">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4.2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4.4000000000000004</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4.5999999999999996</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4.8</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>5.2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>5.4</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>5.6</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>5.8</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>6.2</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>6.4</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>6.6</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>6.8</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>7.2</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>7.4</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>7.6</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>7.8</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>8.1999999999999993</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>8.4</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>8.6</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>8.8000000000000007</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>9</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet3!$B$5:$B$30</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="26"/>
+                <c:pt idx="0">
+                  <c:v>285147</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>126914.8</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>78297.100000000006</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>55346.239999999998</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>41857.54</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>32757</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>26697.52</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>22015.37</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>18392.310000000001</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>15505.26</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>13151</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>11194.16</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>9542.1659999999993</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>8129.0129999999999</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>6906.3419999999996</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>5838</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>4896.6909999999998</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>4060.9009999999998</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>3313.8420000000001</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>2642.1610000000001</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>2034</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>1483.35</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>980.08209999999997</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>519.0521</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>95.156949999999995</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>2.66</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-D165-4768-B04B-56532A7B5FC1}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="2142772767"/>
+        <c:axId val="96401663"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="2142772767"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:min val="4"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="96401663"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="96401663"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="2142772767"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
             <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" spc="120" normalizeH="0" baseline="0">
               <a:solidFill>
                 <a:schemeClr val="tx1">
@@ -4633,6 +5092,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors6.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
@@ -6702,6 +7201,522 @@
 </file>
 
 <file path=xl/charts/style5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style6.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="241">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -7371,6 +8386,47 @@
 </file>
 
 <file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>219075</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>304799</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{95B10557-DF7E-488F-B7F1-3C5DF1FB8709}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -7710,7 +8766,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7288C5F0-AF61-4E26-9BFE-C4E1DAB9DA45}">
   <dimension ref="A2:V47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G25" workbookViewId="0">
+    <sheetView topLeftCell="G25" workbookViewId="0">
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
@@ -8727,6 +9783,269 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D30EFE3F-6A59-4783-AA79-CB31DEB1F652}">
+  <dimension ref="A2:E31"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H27" sqref="H27"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>4000000</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>4000000</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <v>4000000</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5">
+        <v>285147</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>4.2</v>
+      </c>
+      <c r="B6">
+        <v>126914.8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="B7">
+        <v>78297.100000000006</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="B8">
+        <v>55346.239999999998</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>4.8</v>
+      </c>
+      <c r="B9">
+        <v>41857.54</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>5</v>
+      </c>
+      <c r="B10">
+        <v>32757</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>5.2</v>
+      </c>
+      <c r="B11">
+        <v>26697.52</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>5.4</v>
+      </c>
+      <c r="B12">
+        <v>22015.37</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>5.6</v>
+      </c>
+      <c r="B13">
+        <v>18392.310000000001</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>5.8</v>
+      </c>
+      <c r="B14">
+        <v>15505.26</v>
+      </c>
+      <c r="E14">
+        <v>4.9528699999999999</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>6</v>
+      </c>
+      <c r="B15">
+        <v>13151</v>
+      </c>
+      <c r="E15">
+        <f>(50000/E14) -10000</f>
+        <v>95.156949405092746</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>6.2</v>
+      </c>
+      <c r="B16">
+        <v>11194.16</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>6.4</v>
+      </c>
+      <c r="B17">
+        <v>9542.1659999999993</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>6.6</v>
+      </c>
+      <c r="B18">
+        <v>8129.0129999999999</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>6.8</v>
+      </c>
+      <c r="B19">
+        <v>6906.3419999999996</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>7</v>
+      </c>
+      <c r="B20">
+        <v>5838</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>7.2</v>
+      </c>
+      <c r="B21">
+        <v>4896.6909999999998</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>7.4</v>
+      </c>
+      <c r="B22">
+        <v>4060.9009999999998</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>7.6</v>
+      </c>
+      <c r="B23">
+        <v>3313.8420000000001</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>7.8</v>
+      </c>
+      <c r="B24">
+        <v>2642.1610000000001</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>8</v>
+      </c>
+      <c r="B25">
+        <v>2034</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>8.1999999999999993</v>
+      </c>
+      <c r="B26">
+        <v>1483.35</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>8.4</v>
+      </c>
+      <c r="B27">
+        <v>980.08209999999997</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>8.6</v>
+      </c>
+      <c r="B28">
+        <v>519.0521</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>8.8000000000000007</v>
+      </c>
+      <c r="B29">
+        <v>95.156949999999995</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>9</v>
+      </c>
+      <c r="B30">
+        <v>2.66</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>10</v>
+      </c>
+      <c r="B31">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7A581574-D065-4677-A136-CE1820FEC8BC}">
   <dimension ref="A5:F51"/>
   <sheetViews>

</xml_diff>

<commit_message>
Not much in the way of report writing but chnaged ref voltage circuit
Now detects all the way along the rail
</commit_message>
<xml_diff>
--- a/50kHz measurments.xlsx
+++ b/50kHz measurments.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ksmall1\Documents\GitHub\PROJ324_SK\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC7A53D7-43B7-4B24-AFEB-25AA4D163D43}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17DD844A-028C-4C07-9200-197B9BC2D45F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{49929126-E106-4BA5-BBBE-362DD2DFA756}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{49929126-E106-4BA5-BBBE-362DD2DFA756}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,6 +24,10 @@
     </ext>
   </extLst>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -4888,6 +4892,435 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet2!$H$5:$H$23</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="19"/>
+                <c:pt idx="0">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>45</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>55</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>65</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>75</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>85</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>95</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet2!$M$5:$M$23</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="19"/>
+                <c:pt idx="0">
+                  <c:v>216.53699999999998</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>250.25400000000002</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>273.29200000000014</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>317.12099999999987</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>321.51499999999987</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>305.85900000000015</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>315.85099999999989</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>333.5659999999998</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>350.10399999999981</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>319.779</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>382.53700000000026</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>392.80200000000013</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>358.00300000000016</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>370.48100000000022</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>414.05199999999968</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>374.21200000000044</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>342.58200000000033</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>362.73199999999997</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-0485-4BF6-918C-4607AEC7E3EA}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="37185807"/>
+        <c:axId val="46128879"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="37185807"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="46128879"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="46128879"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="37185807"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -5128,6 +5561,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors7.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
@@ -8228,6 +8701,522 @@
     <cs:fontRef idx="minor">
       <a:schemeClr val="dk1"/>
     </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style7.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
   </cs:wall>
 </cs:chartStyle>
 </file>
@@ -8460,6 +9449,42 @@
     </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>171450</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>61912</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>476250</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>138112</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{63993162-7E3D-4F5C-8EC1-F3323BFE52AA}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -8762,7 +9787,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7288C5F0-AF61-4E26-9BFE-C4E1DAB9DA45}">
   <dimension ref="A2:V47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G43" workbookViewId="0">
+    <sheetView topLeftCell="A7" workbookViewId="0">
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
@@ -10043,15 +11068,15 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7A581574-D065-4677-A136-CE1820FEC8BC}">
-  <dimension ref="A5:F51"/>
+  <dimension ref="A5:M51"/>
   <sheetViews>
-    <sheetView topLeftCell="K9" workbookViewId="0">
-      <selection activeCell="F52" sqref="F52"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="O19" sqref="O19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>291.54500000000002</v>
       </c>
@@ -10065,8 +11090,28 @@
       <c r="D5">
         <v>5</v>
       </c>
+      <c r="H5">
+        <v>5</v>
+      </c>
+      <c r="I5">
+        <v>291.54500000000002</v>
+      </c>
+      <c r="J5">
+        <v>528.43399999999997</v>
+      </c>
+      <c r="K5">
+        <f>J5-I5</f>
+        <v>236.88899999999995</v>
+      </c>
+      <c r="L5">
+        <v>508.08199999999999</v>
+      </c>
+      <c r="M5">
+        <f>L5-I5</f>
+        <v>216.53699999999998</v>
+      </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>349.85399999999998</v>
       </c>
@@ -10080,8 +11125,28 @@
       <c r="D6">
         <v>6</v>
       </c>
+      <c r="H6">
+        <v>10</v>
+      </c>
+      <c r="I6">
+        <v>583.09</v>
+      </c>
+      <c r="J6">
+        <v>830.47500000000002</v>
+      </c>
+      <c r="K6">
+        <f t="shared" ref="K6:K16" si="1">J6-I6</f>
+        <v>247.38499999999999</v>
+      </c>
+      <c r="L6">
+        <v>833.34400000000005</v>
+      </c>
+      <c r="M6">
+        <f t="shared" ref="M6:M22" si="2">L6-I6</f>
+        <v>250.25400000000002</v>
+      </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>408.16300000000001</v>
       </c>
@@ -10095,8 +11160,28 @@
       <c r="D7">
         <v>7</v>
       </c>
+      <c r="H7">
+        <v>15</v>
+      </c>
+      <c r="I7">
+        <v>874.63599999999997</v>
+      </c>
+      <c r="J7">
+        <v>1128.7070000000001</v>
+      </c>
+      <c r="K7">
+        <f t="shared" si="1"/>
+        <v>254.07100000000014</v>
+      </c>
+      <c r="L7">
+        <v>1147.9280000000001</v>
+      </c>
+      <c r="M7">
+        <f t="shared" si="2"/>
+        <v>273.29200000000014</v>
+      </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>466.47199999999998</v>
       </c>
@@ -10110,8 +11195,28 @@
       <c r="D8">
         <v>8</v>
       </c>
+      <c r="H8">
+        <v>20</v>
+      </c>
+      <c r="I8">
+        <v>1166.181</v>
+      </c>
+      <c r="J8">
+        <v>1463.9690000000001</v>
+      </c>
+      <c r="K8">
+        <f t="shared" si="1"/>
+        <v>297.78800000000001</v>
+      </c>
+      <c r="L8">
+        <v>1483.3019999999999</v>
+      </c>
+      <c r="M8">
+        <f t="shared" si="2"/>
+        <v>317.12099999999987</v>
+      </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>524.78099999999995</v>
       </c>
@@ -10125,8 +11230,28 @@
       <c r="D9">
         <v>9</v>
       </c>
+      <c r="H9">
+        <v>25</v>
+      </c>
+      <c r="I9">
+        <v>1457.7260000000001</v>
+      </c>
+      <c r="J9">
+        <v>1754.7170000000001</v>
+      </c>
+      <c r="K9">
+        <f t="shared" si="1"/>
+        <v>296.99099999999999</v>
+      </c>
+      <c r="L9">
+        <v>1779.241</v>
+      </c>
+      <c r="M9">
+        <f t="shared" si="2"/>
+        <v>321.51499999999987</v>
+      </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>583.09</v>
       </c>
@@ -10147,8 +11272,28 @@
         <f>E10-A10</f>
         <v>195.10199999999998</v>
       </c>
+      <c r="H10">
+        <v>30</v>
+      </c>
+      <c r="I10">
+        <v>1749.271</v>
+      </c>
+      <c r="J10">
+        <v>2091.2919999999999</v>
+      </c>
+      <c r="K10">
+        <f t="shared" si="1"/>
+        <v>342.02099999999996</v>
+      </c>
+      <c r="L10">
+        <v>2055.13</v>
+      </c>
+      <c r="M10">
+        <f t="shared" si="2"/>
+        <v>305.85900000000015</v>
+      </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>641.399</v>
       </c>
@@ -10166,11 +11311,31 @@
         <v>857.91</v>
       </c>
       <c r="F11">
-        <f t="shared" ref="F11:F50" si="1">E11-A11</f>
+        <f t="shared" ref="F11:F50" si="3">E11-A11</f>
         <v>216.51099999999997</v>
       </c>
+      <c r="H11">
+        <v>35</v>
+      </c>
+      <c r="I11">
+        <v>2040.816</v>
+      </c>
+      <c r="J11">
+        <v>2378.5050000000001</v>
+      </c>
+      <c r="K11">
+        <f t="shared" si="1"/>
+        <v>337.68900000000008</v>
+      </c>
+      <c r="L11">
+        <v>2356.6669999999999</v>
+      </c>
+      <c r="M11">
+        <f t="shared" si="2"/>
+        <v>315.85099999999989</v>
+      </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>699.70799999999997</v>
       </c>
@@ -10188,11 +11353,31 @@
         <v>930.92</v>
       </c>
       <c r="F12">
+        <f t="shared" si="3"/>
+        <v>231.21199999999999</v>
+      </c>
+      <c r="H12">
+        <v>40</v>
+      </c>
+      <c r="I12">
+        <v>2332.3620000000001</v>
+      </c>
+      <c r="J12">
+        <v>2697.9479999999999</v>
+      </c>
+      <c r="K12">
         <f t="shared" si="1"/>
-        <v>231.21199999999999</v>
+        <v>365.58599999999979</v>
+      </c>
+      <c r="L12">
+        <v>2665.9279999999999</v>
+      </c>
+      <c r="M12">
+        <f t="shared" si="2"/>
+        <v>333.5659999999998</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>758.01700000000005</v>
       </c>
@@ -10210,11 +11395,31 @@
         <v>998.04</v>
       </c>
       <c r="F13">
+        <f t="shared" si="3"/>
+        <v>240.02299999999991</v>
+      </c>
+      <c r="H13">
+        <v>45</v>
+      </c>
+      <c r="I13">
+        <v>2623.9070000000002</v>
+      </c>
+      <c r="J13">
+        <v>2993.0309999999999</v>
+      </c>
+      <c r="K13">
         <f t="shared" si="1"/>
-        <v>240.02299999999991</v>
+        <v>369.1239999999998</v>
+      </c>
+      <c r="L13">
+        <v>2974.011</v>
+      </c>
+      <c r="M13">
+        <f t="shared" si="2"/>
+        <v>350.10399999999981</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>816.327</v>
       </c>
@@ -10232,11 +11437,31 @@
         <v>1060.576</v>
       </c>
       <c r="F14">
+        <f t="shared" si="3"/>
+        <v>244.24900000000002</v>
+      </c>
+      <c r="H14">
+        <v>50</v>
+      </c>
+      <c r="I14">
+        <v>2915.4520000000002</v>
+      </c>
+      <c r="J14">
+        <v>3335.5059999999999</v>
+      </c>
+      <c r="K14">
         <f t="shared" si="1"/>
-        <v>244.24900000000002</v>
+        <v>420.05399999999963</v>
+      </c>
+      <c r="L14">
+        <v>3235.2310000000002</v>
+      </c>
+      <c r="M14">
+        <f t="shared" si="2"/>
+        <v>319.779</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>874.63599999999997</v>
       </c>
@@ -10254,11 +11479,31 @@
         <v>1119.93</v>
       </c>
       <c r="F15">
+        <f t="shared" si="3"/>
+        <v>245.2940000000001</v>
+      </c>
+      <c r="H15">
+        <v>55</v>
+      </c>
+      <c r="I15">
+        <v>3206.9969999999998</v>
+      </c>
+      <c r="J15">
+        <v>3667.7449999999999</v>
+      </c>
+      <c r="K15">
         <f t="shared" si="1"/>
-        <v>245.2940000000001</v>
+        <v>460.74800000000005</v>
+      </c>
+      <c r="L15">
+        <v>3589.5340000000001</v>
+      </c>
+      <c r="M15">
+        <f t="shared" si="2"/>
+        <v>382.53700000000026</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>932.94500000000005</v>
       </c>
@@ -10276,11 +11521,31 @@
         <v>1155.1110000000001</v>
       </c>
       <c r="F16">
+        <f t="shared" si="3"/>
+        <v>222.16600000000005</v>
+      </c>
+      <c r="H16">
+        <v>60</v>
+      </c>
+      <c r="I16">
+        <v>3498.5419999999999</v>
+      </c>
+      <c r="J16">
+        <v>3896.4459999999999</v>
+      </c>
+      <c r="K16">
         <f t="shared" si="1"/>
-        <v>222.16600000000005</v>
+        <v>397.904</v>
+      </c>
+      <c r="L16">
+        <v>3891.3440000000001</v>
+      </c>
+      <c r="M16">
+        <f t="shared" si="2"/>
+        <v>392.80200000000013</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>991.25400000000002</v>
       </c>
@@ -10298,11 +11563,31 @@
         <v>1196.798</v>
       </c>
       <c r="F17">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>205.54399999999998</v>
       </c>
+      <c r="H17">
+        <v>65</v>
+      </c>
+      <c r="I17">
+        <v>3790.087</v>
+      </c>
+      <c r="J17">
+        <v>4517.4629999999997</v>
+      </c>
+      <c r="K17">
+        <f>J17-I18</f>
+        <v>436.29999999999973</v>
+      </c>
+      <c r="L17">
+        <v>4148.09</v>
+      </c>
+      <c r="M17">
+        <f>L17-I17</f>
+        <v>358.00300000000016</v>
+      </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>1049.5630000000001</v>
       </c>
@@ -10320,11 +11605,28 @@
         <v>1268.2919999999999</v>
       </c>
       <c r="F18">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>218.72899999999981</v>
       </c>
+      <c r="H18">
+        <v>70</v>
+      </c>
+      <c r="I18">
+        <v>4081.163</v>
+      </c>
+      <c r="K18">
+        <f>AVERAGE(K5:K17)</f>
+        <v>343.27307692307687</v>
+      </c>
+      <c r="L18">
+        <v>4451.6440000000002</v>
+      </c>
+      <c r="M18">
+        <f t="shared" ref="M18:M23" si="4">L18-I18</f>
+        <v>370.48100000000022</v>
+      </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>1107.8720000000001</v>
       </c>
@@ -10342,11 +11644,24 @@
         <v>1323.758</v>
       </c>
       <c r="F19">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>215.88599999999997</v>
       </c>
+      <c r="H19">
+        <v>75</v>
+      </c>
+      <c r="I19">
+        <v>4373.1790000000001</v>
+      </c>
+      <c r="L19">
+        <v>4787.2309999999998</v>
+      </c>
+      <c r="M19">
+        <f t="shared" si="4"/>
+        <v>414.05199999999968</v>
+      </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>1166.181</v>
       </c>
@@ -10364,11 +11679,24 @@
         <v>1418.777</v>
       </c>
       <c r="F20">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>252.596</v>
       </c>
+      <c r="H20">
+        <v>80</v>
+      </c>
+      <c r="I20">
+        <v>4664.723</v>
+      </c>
+      <c r="L20">
+        <v>5038.9350000000004</v>
+      </c>
+      <c r="M20">
+        <f t="shared" si="4"/>
+        <v>374.21200000000044</v>
+      </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>1224.49</v>
       </c>
@@ -10386,11 +11714,24 @@
         <v>1474.5650000000001</v>
       </c>
       <c r="F21">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>250.07500000000005</v>
       </c>
+      <c r="H21">
+        <v>85</v>
+      </c>
+      <c r="I21">
+        <v>4956.268</v>
+      </c>
+      <c r="L21">
+        <v>5298.85</v>
+      </c>
+      <c r="M21">
+        <f t="shared" si="4"/>
+        <v>342.58200000000033</v>
+      </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>1282.799</v>
       </c>
@@ -10408,11 +11749,15 @@
         <v>1568.586</v>
       </c>
       <c r="F22">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>285.78700000000003</v>
       </c>
+      <c r="M22">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>1341.1079999999999</v>
       </c>
@@ -10430,11 +11775,24 @@
         <v>1639.94</v>
       </c>
       <c r="F23">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>298.83200000000011</v>
       </c>
+      <c r="H23">
+        <v>95</v>
+      </c>
+      <c r="I23">
+        <v>5539.3590000000004</v>
+      </c>
+      <c r="L23">
+        <v>5902.0910000000003</v>
+      </c>
+      <c r="M23">
+        <f t="shared" si="4"/>
+        <v>362.73199999999997</v>
+      </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>1399.4169999999999</v>
       </c>
@@ -10452,11 +11810,19 @@
         <v>1704.5150000000001</v>
       </c>
       <c r="F24">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>305.09800000000018</v>
       </c>
+      <c r="L24">
+        <f>AVERAGE(L5:L23)</f>
+        <v>3119.254611111111</v>
+      </c>
+      <c r="M24">
+        <f>AVERAGE(M5:M23)</f>
+        <v>315.85678947368427</v>
+      </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>1457.7260000000001</v>
       </c>
@@ -10474,11 +11840,11 @@
         <v>1773.2639999999999</v>
       </c>
       <c r="F25">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>315.53799999999978</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>1516.0350000000001</v>
       </c>
@@ -10496,11 +11862,11 @@
         <v>1817.5250000000001</v>
       </c>
       <c r="F26">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>301.49</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>1574.3440000000001</v>
       </c>
@@ -10518,11 +11884,11 @@
         <v>1874.587</v>
       </c>
       <c r="F27">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>300.24299999999994</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>1632.653</v>
       </c>
@@ -10540,11 +11906,11 @@
         <v>1911.2529999999999</v>
       </c>
       <c r="F28">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>278.59999999999991</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>1690.962</v>
       </c>
@@ -10562,11 +11928,11 @@
         <v>1954.374</v>
       </c>
       <c r="F29">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>263.41200000000003</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>1749.271</v>
       </c>
@@ -10584,11 +11950,11 @@
         <v>2033.759</v>
       </c>
       <c r="F30">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>284.48800000000006</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>1807.58</v>
       </c>
@@ -10606,11 +11972,11 @@
         <v>2091.7370000000001</v>
       </c>
       <c r="F31">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>284.15700000000015</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>1865.8889999999999</v>
       </c>
@@ -10628,7 +11994,7 @@
         <v>2186.4340000000002</v>
       </c>
       <c r="F32">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>320.5450000000003</v>
       </c>
     </row>
@@ -10650,7 +12016,7 @@
         <v>2267.799</v>
       </c>
       <c r="F33">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>343.60099999999989</v>
       </c>
     </row>
@@ -10672,7 +12038,7 @@
         <v>2346.9789999999998</v>
       </c>
       <c r="F34">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>364.47199999999975</v>
       </c>
     </row>
@@ -10694,7 +12060,7 @@
         <v>2425.759</v>
       </c>
       <c r="F35">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>384.94299999999998</v>
       </c>
     </row>
@@ -10716,7 +12082,7 @@
         <v>2448.9490000000001</v>
       </c>
       <c r="F36">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>349.82400000000007</v>
       </c>
     </row>
@@ -10738,7 +12104,7 @@
         <v>2480.98</v>
       </c>
       <c r="F37">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>323.54599999999982</v>
       </c>
     </row>
@@ -10760,7 +12126,7 @@
         <v>2521.2939999999999</v>
       </c>
       <c r="F38">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>305.55099999999993</v>
       </c>
     </row>
@@ -10782,7 +12148,7 @@
         <v>2590.4650000000001</v>
       </c>
       <c r="F39">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>316.41300000000001</v>
       </c>
     </row>
@@ -10804,7 +12170,7 @@
         <v>2640.1909999999998</v>
       </c>
       <c r="F40">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>307.82899999999972</v>
       </c>
     </row>
@@ -10826,7 +12192,7 @@
         <v>2710.616</v>
       </c>
       <c r="F41">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>319.94500000000016</v>
       </c>
     </row>
@@ -10848,7 +12214,7 @@
         <v>2763.4740000000002</v>
       </c>
       <c r="F42">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>314.49400000000014</v>
       </c>
     </row>
@@ -10870,7 +12236,7 @@
         <v>2845.0210000000002</v>
       </c>
       <c r="F43">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>337.73199999999997</v>
       </c>
     </row>
@@ -10892,7 +12258,7 @@
         <v>2930.0509999999999</v>
       </c>
       <c r="F44">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>364.45299999999997</v>
       </c>
     </row>
@@ -10911,7 +12277,7 @@
         <v>3050.4340000000002</v>
       </c>
       <c r="F45">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>426.52700000000004</v>
       </c>
     </row>
@@ -10926,7 +12292,7 @@
         <v>3280.0010000000002</v>
       </c>
       <c r="F46">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>364.54899999999998</v>
       </c>
     </row>
@@ -10941,7 +12307,7 @@
         <v>3565.1909999999998</v>
       </c>
       <c r="F47">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>358.19399999999996</v>
       </c>
     </row>
@@ -10956,7 +12322,7 @@
         <v>3884.2820000000002</v>
       </c>
       <c r="F48">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>385.74000000000024</v>
       </c>
     </row>
@@ -10971,7 +12337,7 @@
         <v>4165.6670000000004</v>
       </c>
       <c r="F49">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>375.58000000000038</v>
       </c>
     </row>
@@ -10986,7 +12352,7 @@
         <v>4498.4449999999997</v>
       </c>
       <c r="F50">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>416.8119999999999</v>
       </c>
     </row>

</xml_diff>

<commit_message>
More words + Started adding Figures
</commit_message>
<xml_diff>
--- a/50kHz measurments.xlsx
+++ b/50kHz measurments.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20348"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ksmall1\Documents\GitHub\PROJ324_SK\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kiera\Documents\GitHub\PROJ324_SK\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF2845CF-8169-4306-B237-7379EF127A0E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{780CB8F2-9EA1-407C-96B2-6EECAFEE39AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{49929126-E106-4BA5-BBBE-362DD2DFA756}"/>
   </bookViews>
@@ -23,6 +23,17 @@
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -3030,6 +3041,19 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:minorGridlines>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="5000"/>
+                  <a:lumOff val="95000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:minorGridlines>
         <c:title>
           <c:tx>
             <c:rich>
@@ -3153,6 +3177,19 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:minorGridlines>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="5000"/>
+                  <a:lumOff val="95000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:minorGridlines>
         <c:title>
           <c:tx>
             <c:rich>
@@ -3304,6 +3341,7 @@
     <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
     <c:pageSetup/>
   </c:printSettings>
+  <c:userShapes r:id="rId3"/>
 </c:chartSpace>
 </file>
 
@@ -16991,15 +17029,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>271462</xdr:colOff>
+      <xdr:colOff>309561</xdr:colOff>
       <xdr:row>69</xdr:row>
-      <xdr:rowOff>100011</xdr:rowOff>
+      <xdr:rowOff>119061</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>21</xdr:col>
-      <xdr:colOff>95250</xdr:colOff>
-      <xdr:row>93</xdr:row>
-      <xdr:rowOff>123824</xdr:rowOff>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>104774</xdr:colOff>
+      <xdr:row>94</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -17025,6 +17063,517 @@
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing6.xml><?xml version="1.0" encoding="utf-8"?>
+<c:userShapes xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart">
+  <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
+    <cdr:from>
+      <cdr:x>0.2409</cdr:x>
+      <cdr:y>0.05799</cdr:y>
+    </cdr:from>
+    <cdr:to>
+      <cdr:x>0.2419</cdr:x>
+      <cdr:y>0.98779</cdr:y>
+    </cdr:to>
+    <cdr:cxnSp macro="">
+      <cdr:nvCxnSpPr>
+        <cdr:cNvPr id="3" name="Straight Connector 2">
+          <a:extLst xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5F3E167A-9F44-28BD-D94A-9199BBCFB722}"/>
+            </a:ext>
+          </a:extLst>
+        </cdr:cNvPr>
+        <cdr:cNvCxnSpPr/>
+      </cdr:nvCxnSpPr>
+      <cdr:spPr>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:off x="2300289" y="271464"/>
+          <a:ext cx="9525" cy="4352925"/>
+        </a:xfrm>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" w="19050"/>
+      </cdr:spPr>
+      <cdr:style>
+        <a:lnRef xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" idx="1">
+          <a:schemeClr val="accent2"/>
+        </a:lnRef>
+        <a:fillRef xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:fillRef>
+        <a:effectRef xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:effectRef>
+        <a:fontRef xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </cdr:style>
+    </cdr:cxnSp>
+  </cdr:relSizeAnchor>
+  <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
+    <cdr:from>
+      <cdr:x>0.63973</cdr:x>
+      <cdr:y>0.06172</cdr:y>
+    </cdr:from>
+    <cdr:to>
+      <cdr:x>0.64073</cdr:x>
+      <cdr:y>0.99152</cdr:y>
+    </cdr:to>
+    <cdr:cxnSp macro="">
+      <cdr:nvCxnSpPr>
+        <cdr:cNvPr id="4" name="Straight Connector 3">
+          <a:extLst xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{795861CF-B037-B569-A7FE-1D9BD0F58DAB}"/>
+            </a:ext>
+          </a:extLst>
+        </cdr:cNvPr>
+        <cdr:cNvCxnSpPr/>
+      </cdr:nvCxnSpPr>
+      <cdr:spPr>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:off x="6108700" y="288925"/>
+          <a:ext cx="9525" cy="4352925"/>
+        </a:xfrm>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" w="19050"/>
+      </cdr:spPr>
+      <cdr:style>
+        <a:lnRef xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" idx="1">
+          <a:schemeClr val="accent2"/>
+        </a:lnRef>
+        <a:fillRef xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:fillRef>
+        <a:effectRef xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:effectRef>
+        <a:fontRef xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </cdr:style>
+    </cdr:cxnSp>
+  </cdr:relSizeAnchor>
+  <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
+    <cdr:from>
+      <cdr:x>0.36941</cdr:x>
+      <cdr:y>0.06172</cdr:y>
+    </cdr:from>
+    <cdr:to>
+      <cdr:x>0.37041</cdr:x>
+      <cdr:y>0.99152</cdr:y>
+    </cdr:to>
+    <cdr:cxnSp macro="">
+      <cdr:nvCxnSpPr>
+        <cdr:cNvPr id="5" name="Straight Connector 4">
+          <a:extLst xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{795861CF-B037-B569-A7FE-1D9BD0F58DAB}"/>
+            </a:ext>
+          </a:extLst>
+        </cdr:cNvPr>
+        <cdr:cNvCxnSpPr/>
+      </cdr:nvCxnSpPr>
+      <cdr:spPr>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:off x="3527425" y="288925"/>
+          <a:ext cx="9525" cy="4352925"/>
+        </a:xfrm>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" w="19050"/>
+      </cdr:spPr>
+      <cdr:style>
+        <a:lnRef xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" idx="1">
+          <a:schemeClr val="accent2"/>
+        </a:lnRef>
+        <a:fillRef xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:fillRef>
+        <a:effectRef xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:effectRef>
+        <a:fontRef xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </cdr:style>
+    </cdr:cxnSp>
+  </cdr:relSizeAnchor>
+  <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
+    <cdr:from>
+      <cdr:x>0.12219</cdr:x>
+      <cdr:y>0.0824</cdr:y>
+    </cdr:from>
+    <cdr:to>
+      <cdr:x>0.17107</cdr:x>
+      <cdr:y>0.13733</cdr:y>
+    </cdr:to>
+    <cdr:sp macro="" textlink="">
+      <cdr:nvSpPr>
+        <cdr:cNvPr id="6" name="TextBox 5">
+          <a:extLst xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FE2F8412-D0F7-B02A-698F-B02F9C279DE3}"/>
+            </a:ext>
+          </a:extLst>
+        </cdr:cNvPr>
+        <cdr:cNvSpPr txBox="1"/>
+      </cdr:nvSpPr>
+      <cdr:spPr>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:off x="1166814" y="385764"/>
+          <a:ext cx="466725" cy="257175"/>
+        </a:xfrm>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:schemeClr val="accent2"/>
+        </a:solidFill>
+      </cdr:spPr>
+      <cdr:txBody>
+        <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" vertOverflow="clip" wrap="square" rtlCol="0"/>
+        <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100" b="1"/>
+            <a:t>-250</a:t>
+          </a:r>
+        </a:p>
+      </cdr:txBody>
+    </cdr:sp>
+  </cdr:relSizeAnchor>
+  <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
+    <cdr:from>
+      <cdr:x>0.79634</cdr:x>
+      <cdr:y>0.08613</cdr:y>
+    </cdr:from>
+    <cdr:to>
+      <cdr:x>0.84522</cdr:x>
+      <cdr:y>0.14106</cdr:y>
+    </cdr:to>
+    <cdr:sp macro="" textlink="">
+      <cdr:nvSpPr>
+        <cdr:cNvPr id="7" name="TextBox 1">
+          <a:extLst xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5E48EC37-AE4F-DB5B-557B-5112376F4547}"/>
+            </a:ext>
+          </a:extLst>
+        </cdr:cNvPr>
+        <cdr:cNvSpPr txBox="1"/>
+      </cdr:nvSpPr>
+      <cdr:spPr>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:off x="7604125" y="403225"/>
+          <a:ext cx="466725" cy="257175"/>
+        </a:xfrm>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:schemeClr val="accent2"/>
+        </a:solidFill>
+      </cdr:spPr>
+      <cdr:txBody>
+        <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" wrap="square" rtlCol="0"/>
+        <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:lvl1pPr marL="0" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl1pPr>
+          <a:lvl2pPr marL="457200" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl2pPr>
+          <a:lvl3pPr marL="914400" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl3pPr>
+          <a:lvl4pPr marL="1371600" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl4pPr>
+          <a:lvl5pPr marL="1828800" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl5pPr>
+          <a:lvl6pPr marL="2286000" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl6pPr>
+          <a:lvl7pPr marL="2743200" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl7pPr>
+          <a:lvl8pPr marL="3200400" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl8pPr>
+          <a:lvl9pPr marL="3657600" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl9pPr>
+        </a:lstStyle>
+        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100" b="1"/>
+            <a:t>-400</a:t>
+          </a:r>
+        </a:p>
+      </cdr:txBody>
+    </cdr:sp>
+  </cdr:relSizeAnchor>
+  <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
+    <cdr:from>
+      <cdr:x>0.48013</cdr:x>
+      <cdr:y>0.08613</cdr:y>
+    </cdr:from>
+    <cdr:to>
+      <cdr:x>0.52901</cdr:x>
+      <cdr:y>0.14106</cdr:y>
+    </cdr:to>
+    <cdr:sp macro="" textlink="">
+      <cdr:nvSpPr>
+        <cdr:cNvPr id="8" name="TextBox 1">
+          <a:extLst xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5E48EC37-AE4F-DB5B-557B-5112376F4547}"/>
+            </a:ext>
+          </a:extLst>
+        </cdr:cNvPr>
+        <cdr:cNvSpPr txBox="1"/>
+      </cdr:nvSpPr>
+      <cdr:spPr>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:off x="4584700" y="403225"/>
+          <a:ext cx="466725" cy="257175"/>
+        </a:xfrm>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:schemeClr val="accent2"/>
+        </a:solidFill>
+      </cdr:spPr>
+      <cdr:txBody>
+        <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" wrap="square" rtlCol="0"/>
+        <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:lvl1pPr marL="0" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl1pPr>
+          <a:lvl2pPr marL="457200" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl2pPr>
+          <a:lvl3pPr marL="914400" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl3pPr>
+          <a:lvl4pPr marL="1371600" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl4pPr>
+          <a:lvl5pPr marL="1828800" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl5pPr>
+          <a:lvl6pPr marL="2286000" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl6pPr>
+          <a:lvl7pPr marL="2743200" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl7pPr>
+          <a:lvl8pPr marL="3200400" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl8pPr>
+          <a:lvl9pPr marL="3657600" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl9pPr>
+        </a:lstStyle>
+        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100" b="1"/>
+            <a:t>-350</a:t>
+          </a:r>
+        </a:p>
+      </cdr:txBody>
+    </cdr:sp>
+  </cdr:relSizeAnchor>
+  <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
+    <cdr:from>
+      <cdr:x>0.28662</cdr:x>
+      <cdr:y>0.0841</cdr:y>
+    </cdr:from>
+    <cdr:to>
+      <cdr:x>0.33549</cdr:x>
+      <cdr:y>0.13903</cdr:y>
+    </cdr:to>
+    <cdr:sp macro="" textlink="">
+      <cdr:nvSpPr>
+        <cdr:cNvPr id="9" name="TextBox 1">
+          <a:extLst xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5E48EC37-AE4F-DB5B-557B-5112376F4547}"/>
+            </a:ext>
+          </a:extLst>
+        </cdr:cNvPr>
+        <cdr:cNvSpPr txBox="1"/>
+      </cdr:nvSpPr>
+      <cdr:spPr>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:off x="2736850" y="393700"/>
+          <a:ext cx="466725" cy="257175"/>
+        </a:xfrm>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:schemeClr val="accent2"/>
+        </a:solidFill>
+      </cdr:spPr>
+      <cdr:txBody>
+        <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" wrap="square" rtlCol="0"/>
+        <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:lvl1pPr marL="0" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl1pPr>
+          <a:lvl2pPr marL="457200" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl2pPr>
+          <a:lvl3pPr marL="914400" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl3pPr>
+          <a:lvl4pPr marL="1371600" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl4pPr>
+          <a:lvl5pPr marL="1828800" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl5pPr>
+          <a:lvl6pPr marL="2286000" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl6pPr>
+          <a:lvl7pPr marL="2743200" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl7pPr>
+          <a:lvl8pPr marL="3200400" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl8pPr>
+          <a:lvl9pPr marL="3657600" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl9pPr>
+        </a:lstStyle>
+        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100" b="1"/>
+            <a:t>-300</a:t>
+          </a:r>
+        </a:p>
+      </cdr:txBody>
+    </cdr:sp>
+  </cdr:relSizeAnchor>
+</c:userShapes>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -21414,8 +21963,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FE8D9150-10E7-4342-83C2-EC0FE8E58F08}">
   <dimension ref="A3:J80"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="K6" sqref="K6"/>
+    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
+      <selection activeCell="G82" sqref="G82"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>